<commit_message>
pcb adapted + BOM completed
</commit_message>
<xml_diff>
--- a/Hardware/BOM/BOM.xlsx
+++ b/Hardware/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvestr.vankappe\Documents\Telemtetry-for-the-Formula-Student\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A377553-1455-4827-AB86-05CDF04F220A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699FC47E-E743-42EC-82E8-FF6EFB93BA7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{C5940FAF-58AE-4B20-8456-6D168406407E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="213">
   <si>
     <t>Nbr.</t>
   </si>
@@ -626,9 +626,6 @@
     <t>Asus</t>
   </si>
   <si>
-    <t>Routeur RT-AX86U Pro</t>
-  </si>
-  <si>
     <t xml:space="preserve">	490-4982-ND</t>
   </si>
   <si>
@@ -636,6 +633,39 @@
   </si>
   <si>
     <t>Microwave Coaxial adapter</t>
+  </si>
+  <si>
+    <t>Distrelec</t>
+  </si>
+  <si>
+    <t>Taoglas</t>
+  </si>
+  <si>
+    <t>Wifi Router - Asus RT-AX86U Pro</t>
+  </si>
+  <si>
+    <t>302-20-253</t>
+  </si>
+  <si>
+    <t>Dual Band wifi antenna</t>
+  </si>
+  <si>
+    <t>301-31-595</t>
+  </si>
+  <si>
+    <t>Nedis</t>
+  </si>
+  <si>
+    <t>Antenna cable SMA 2m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	ADP-SMAM-RPSF-G-ND</t>
+  </si>
+  <si>
+    <t>Linx Technologies</t>
+  </si>
+  <si>
+    <t>SMA to RP-SMA adapter</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396F9A50-D1DD-4737-BBCD-FCA6E3CA50E5}">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,7 +1877,7 @@
         <v>1.5</v>
       </c>
       <c r="G20" s="16">
-        <f t="shared" ref="G20:G40" si="1">F20*B20</f>
+        <f t="shared" ref="G20:G43" si="1">F20*B20</f>
         <v>1.5</v>
       </c>
       <c r="H20" s="5"/>
@@ -2301,7 +2331,7 @@
         <v>198</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F39" s="4">
         <v>247</v>
@@ -2312,102 +2342,177 @@
       </c>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>3</v>
+        <v>202</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F40" s="4">
-        <v>27.7</v>
+        <v>15.64</v>
       </c>
       <c r="G40" s="16">
         <f t="shared" si="1"/>
+        <v>15.64</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.72</v>
+      </c>
+      <c r="G41" s="16">
+        <f t="shared" si="1"/>
+        <v>6.72</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="4">
+        <v>10.29</v>
+      </c>
+      <c r="G42" s="16">
+        <f t="shared" si="1"/>
+        <v>10.29</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F43" s="4">
         <v>27.7</v>
       </c>
-      <c r="H40" s="5"/>
-      <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
+      <c r="G43" s="16">
+        <f t="shared" si="1"/>
+        <v>27.7</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="K43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="29"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="9">
-        <v>1</v>
-      </c>
-      <c r="C42" s="10" t="s">
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F45" s="12">
         <v>130</v>
       </c>
-      <c r="G42" s="16">
-        <f t="shared" ref="G42" si="2">F42*B42</f>
+      <c r="G45" s="16">
+        <f t="shared" ref="G45" si="2">F45*B45</f>
         <v>130</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-    </row>
-    <row r="44" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="35" t="s">
+      <c r="H45" s="13"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+    </row>
+    <row r="47" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="15">
-        <f>SUM(G3:G42)</f>
-        <v>596.53399999999988</v>
+      <c r="F47" s="35"/>
+      <c r="G47" s="15">
+        <f>SUM(G3:G45)</f>
+        <v>629.18399999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A44:H44"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A46:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3194,15 +3299,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9f964f78-7045-481f-8f08-bb22d56de14e" xsi:nil="true"/>
@@ -3218,6 +3314,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3240,14 +3345,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F8BD0A9-1453-4AF8-8CA7-9D3A6DF72AF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3256,4 +3353,12 @@
     <ds:schemaRef ds:uri="59352aba-b979-4180-93b6-1b29a58e7092"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
BOM update (inductore wirewound + RF in 1005)
</commit_message>
<xml_diff>
--- a/Hardware/BOM/BOM.xlsx
+++ b/Hardware/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvestr.vankappe\Documents\Telemtetry-for-the-Formula-Student\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699FC47E-E743-42EC-82E8-FF6EFB93BA7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C248FC-C9DA-4937-8E47-22E10585D6A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{C5940FAF-58AE-4B20-8456-6D168406407E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="215">
   <si>
     <t>Nbr.</t>
   </si>
@@ -410,24 +410,12 @@
     <t>Capacitor 1608 - 4.7 nF</t>
   </si>
   <si>
-    <t>Capacitor 1608 - 10 nF</t>
-  </si>
-  <si>
-    <t>Capacitor 1608 - 47 pF</t>
-  </si>
-  <si>
     <t>4 Layer PCB</t>
   </si>
   <si>
-    <t>80-CBR06C470J5GAUTO</t>
-  </si>
-  <si>
     <t>80-C0603X472K5GAUTO</t>
   </si>
   <si>
-    <t>80-C0603C103KARAUTO</t>
-  </si>
-  <si>
     <t>Capacitor 3216 - 10 uF</t>
   </si>
   <si>
@@ -473,12 +461,6 @@
     <t>EMC Choke</t>
   </si>
   <si>
-    <t>High Frequency Inductor 1608 - 27 nH</t>
-  </si>
-  <si>
-    <t>871-B82496C3270G000</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -666,6 +648,30 @@
   </si>
   <si>
     <t>SMA to RP-SMA adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-0402DC-27NXGRW </t>
+  </si>
+  <si>
+    <t>RF Inductor, Wirewound, 1005 - 27 nH</t>
+  </si>
+  <si>
+    <t>Coilcraft</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>Capacitor 1005 - 10 nF</t>
+  </si>
+  <si>
+    <t>Capacitor 1005 - 47 pF</t>
+  </si>
+  <si>
+    <t>810-C1005X7R1H103KBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">810-C1005C0G1H470G </t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1382,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1427,7 @@
     </row>
     <row r="2" spans="1:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -1453,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>122</v>
@@ -1535,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>122</v>
@@ -1562,20 +1568,20 @@
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>132</v>
+        <v>213</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="F8" s="4">
-        <v>0.8</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>17</v>
@@ -1589,20 +1595,20 @@
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
       <c r="F9" s="4">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>17</v>
@@ -1616,13 +1622,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>122</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F10" s="4">
         <v>0.41</v>
@@ -1645,13 +1651,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F11" s="4">
         <v>0.44</v>
@@ -1672,13 +1678,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F12" s="4">
         <v>0.5</v>
@@ -1699,13 +1705,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F13" s="4">
         <v>0.09</v>
@@ -1726,13 +1732,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F14" s="4">
         <v>2.0699999999999998</v>
@@ -1751,13 +1757,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F15" s="4">
         <v>6.23</v>
@@ -1776,24 +1782,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="F16" s="4">
-        <v>0.44600000000000001</v>
+        <v>1.41</v>
       </c>
       <c r="G16" s="16">
         <f t="shared" si="0"/>
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>1.41</v>
+      </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
@@ -1803,13 +1807,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F17" s="4">
         <v>1.17</v>
@@ -1828,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>43</v>
@@ -1865,13 +1869,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F20" s="4">
         <v>1.5</v>
@@ -1890,13 +1894,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F21" s="4">
         <v>1.03</v>
@@ -1916,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>4</v>
@@ -1941,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>96</v>
@@ -1966,13 +1970,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F24" s="4">
         <v>2.97</v>
@@ -1991,13 +1995,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F25" s="4">
         <v>5.75</v>
@@ -2016,10 +2020,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>115</v>
@@ -2041,13 +2045,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F27" s="4">
         <v>0.42799999999999999</v>
@@ -2078,13 +2082,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F29" s="4">
         <v>1.17</v>
@@ -2105,13 +2109,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F30" s="4">
         <v>0.39</v>
@@ -2132,13 +2136,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F31" s="4">
         <v>1.1000000000000001</v>
@@ -2159,13 +2163,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F32" s="4">
         <v>4.0999999999999996</v>
@@ -2184,13 +2188,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F33" s="4">
         <v>1.1200000000000001</v>
@@ -2209,13 +2213,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F34" s="4">
         <v>1.92</v>
@@ -2230,7 +2234,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -2248,13 +2252,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F36" s="4">
         <v>14.85</v>
@@ -2273,13 +2277,13 @@
         <v>1</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F37" s="4">
         <v>57.44</v>
@@ -2300,13 +2304,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F38" s="4">
         <v>55.84</v>
@@ -2319,19 +2323,19 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="F39" s="4">
         <v>247</v>
@@ -2344,19 +2348,19 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B40" s="3">
         <v>1</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F40" s="4">
         <v>15.64</v>
@@ -2375,13 +2379,13 @@
         <v>1</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F41" s="4">
         <v>6.72</v>
@@ -2394,19 +2398,19 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>208</v>
-      </c>
       <c r="E42" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F42" s="4">
         <v>10.29</v>
@@ -2425,13 +2429,13 @@
         <v>1</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F43" s="4">
         <v>27.7</v>
@@ -2470,7 +2474,7 @@
         <v>7</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F45" s="12">
         <v>130</v>
@@ -2494,12 +2498,12 @@
     </row>
     <row r="47" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="35" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F47" s="35"/>
       <c r="G47" s="15">
         <f>SUM(G3:G45)</f>
-        <v>629.18399999999997</v>
+        <v>629.62800000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2524,7 +2528,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C6" sqref="A6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,6 +3303,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9f964f78-7045-481f-8f08-bb22d56de14e" xsi:nil="true"/>
@@ -3314,15 +3327,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3345,6 +3349,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F8BD0A9-1453-4AF8-8CA7-9D3A6DF72AF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3353,12 +3365,4 @@
     <ds:schemaRef ds:uri="59352aba-b979-4180-93b6-1b29a58e7092"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update BOM + bloc diagram
</commit_message>
<xml_diff>
--- a/Hardware/BOM/BOM.xlsx
+++ b/Hardware/BOM/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylve\OneDrive\Bureau\Telemtetry-for-the-Formula-Student\Hardware\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sylvestr.vankappe\Documents\Telemtetry-for-the-Formula-Student\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99BF9CA-0B92-4128-8E0F-C2C2C35469D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB45C6A-451E-46EC-ADE8-F66E99EA3E06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C5940FAF-58AE-4B20-8456-6D168406407E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" xr2:uid="{C5940FAF-58AE-4B20-8456-6D168406407E}"/>
   </bookViews>
   <sheets>
     <sheet name="whole list" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -586,9 +575,6 @@
     <t xml:space="preserve">538-73251-1150 </t>
   </si>
   <si>
-    <t xml:space="preserve">RF Connectors / Coaxial Connectors SMA EDGE MOUNT JACK </t>
-  </si>
-  <si>
     <t>Antennas Multi-band active GNSS antenna - SMA</t>
   </si>
   <si>
@@ -692,6 +678,9 @@
   </si>
   <si>
     <t>Light button</t>
+  </si>
+  <si>
+    <t>SMA connector</t>
   </si>
 </sst>
 </file>
@@ -820,7 +809,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -921,15 +910,15 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -941,39 +930,118 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -995,18 +1063,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1023,9 +1079,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,11 +1114,89 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1085,7 +1216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1381,27 +1512,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396F9A50-D1DD-4737-BBCD-FCA6E3CA50E5}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="28.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="58.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1427,34 +1558,34 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:14" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="26" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3">
@@ -1472,7 +1603,7 @@
       <c r="F4" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="11">
         <f t="shared" ref="G4:G18" si="0">F4*B4</f>
         <v>0.63000000000000012</v>
       </c>
@@ -1481,8 +1612,8 @@
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
@@ -1500,7 +1631,7 @@
       <c r="F5" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
@@ -1508,8 +1639,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3">
@@ -1527,7 +1658,7 @@
       <c r="F6" s="4">
         <v>0.46</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
@@ -1535,8 +1666,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="3">
@@ -1554,7 +1685,7 @@
       <c r="F7" s="4">
         <v>0.4</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
@@ -1562,26 +1693,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="F8" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
@@ -1589,26 +1720,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F9" s="4">
         <v>0.35</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
@@ -1616,8 +1747,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3">
@@ -1635,7 +1766,7 @@
       <c r="F10" s="4">
         <v>0.41</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
@@ -1645,8 +1776,8 @@
       <c r="K10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="3">
@@ -1664,7 +1795,7 @@
       <c r="F11" s="4">
         <v>0.44</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
@@ -1672,8 +1803,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="3">
@@ -1691,7 +1822,7 @@
       <c r="F12" s="4">
         <v>0.5</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="11">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -1699,8 +1830,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3">
@@ -1718,7 +1849,7 @@
       <c r="F13" s="4">
         <v>0.09</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="11">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
@@ -1726,8 +1857,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="3">
@@ -1745,7 +1876,7 @@
       <c r="F14" s="4">
         <v>2.0699999999999998</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="11">
         <f t="shared" si="0"/>
         <v>2.0699999999999998</v>
       </c>
@@ -1753,8 +1884,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="3">
@@ -1772,7 +1903,7 @@
       <c r="F15" s="4">
         <v>6.23</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="11">
         <f t="shared" si="0"/>
         <v>6.23</v>
       </c>
@@ -1780,26 +1911,26 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="F16" s="4">
         <v>1.41</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>1.41</v>
       </c>
@@ -1807,8 +1938,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="3">
@@ -1826,7 +1957,7 @@
       <c r="F17" s="4">
         <v>1.17</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="11">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
@@ -1834,74 +1965,74 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="39">
+        <v>1</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="42">
         <v>0.41</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="43">
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="44">
         <v>45092</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="46">
+        <v>1</v>
+      </c>
+      <c r="C20" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="49">
         <v>1.5</v>
       </c>
-      <c r="G20" s="15">
-        <f t="shared" ref="G20:G44" si="1">F20*B20</f>
+      <c r="G20" s="50">
+        <f t="shared" ref="G20:G45" si="1">F20*B20</f>
         <v>1.5</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="51">
         <v>45092</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="3">
@@ -1919,7 +2050,7 @@
       <c r="F21" s="4">
         <v>1.03</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="11">
         <f t="shared" si="1"/>
         <v>2.06</v>
       </c>
@@ -1928,8 +2059,8 @@
       </c>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
+    <row r="22" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="3">
@@ -1947,7 +2078,7 @@
       <c r="F22" s="4">
         <v>0.42</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="11">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
@@ -1955,8 +2086,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="3">
@@ -1974,7 +2105,7 @@
       <c r="F23" s="4">
         <v>2.5</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="11">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
@@ -1982,8 +2113,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="20" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="3">
@@ -2001,7 +2132,7 @@
       <c r="F24" s="4">
         <v>2.97</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="11">
         <f t="shared" si="1"/>
         <v>2.97</v>
       </c>
@@ -2009,8 +2140,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="3">
@@ -2028,7 +2159,7 @@
       <c r="F25" s="4">
         <v>5.75</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="11">
         <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
@@ -2036,8 +2167,8 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="3">
@@ -2055,7 +2186,7 @@
       <c r="F26" s="4">
         <v>20.67</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="11">
         <f t="shared" si="1"/>
         <v>20.67</v>
       </c>
@@ -2063,537 +2194,547 @@
         <v>45092</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="s">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="39">
+        <v>1</v>
+      </c>
+      <c r="C27" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="42">
         <v>0.42799999999999999</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="43">
         <f t="shared" si="1"/>
         <v>0.42799999999999999</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="44">
         <v>45092</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="57"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F30" s="4">
         <v>1.17</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G30" s="11">
         <f t="shared" si="1"/>
         <v>1.17</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="6" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F31" s="4">
         <v>0.39</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G31" s="11">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F32" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G32" s="11">
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="6" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="E33" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F33" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H33" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="6" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E33" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F33" s="4">
+      <c r="E34" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="4">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>1.1200000000000001</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H34" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="20" t="s">
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B35" s="3">
         <v>2</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E35" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="F35" s="4">
         <v>1.92</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>3.84</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="26" t="s">
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="20" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F37" s="4">
         <v>14.85</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>14.85</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H37" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F38" s="4">
         <v>57.44</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G38" s="11">
         <f t="shared" si="1"/>
         <v>57.44</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H38" s="5">
         <v>45079</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" s="6" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F38" s="4">
+      <c r="E39" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="4">
         <v>55.84</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G39" s="11">
         <f t="shared" si="1"/>
         <v>55.84</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H39" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="20" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F39" s="4">
+      <c r="E40" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" s="4">
         <v>247</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G40" s="11">
         <f t="shared" si="1"/>
         <v>247</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H40" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="6" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E41" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" s="4">
+      <c r="F41" s="4">
         <v>18.95</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G41" s="11">
         <f t="shared" si="1"/>
         <v>18.95</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H41" s="5">
         <v>45106</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="E42" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="F41" s="4">
+      <c r="F42" s="4">
         <v>15.64</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G42" s="11">
         <f t="shared" si="1"/>
         <v>15.64</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H42" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="20" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E43" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="F42" s="4">
+      <c r="F43" s="4">
         <v>6.72</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G43" s="11">
         <f t="shared" si="1"/>
         <v>6.72</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H43" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="6" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E44" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F43" s="4">
+      <c r="F44" s="4">
         <v>10.29</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G44" s="11">
         <f t="shared" si="1"/>
         <v>10.29</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H44" s="5">
         <v>45092</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="20" t="s">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="E45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="F44" s="4">
+      <c r="F45" s="4">
         <v>27.7</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G45" s="11">
         <f t="shared" si="1"/>
         <v>27.7</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H45" s="5">
         <v>45092</v>
       </c>
-      <c r="K44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="26" t="s">
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="28"/>
-      <c r="J45" s="13"/>
-    </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="21" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="23"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="9">
-        <v>1</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="B47" s="32">
+        <v>1</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D47" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E47" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F47" s="35">
         <v>130</v>
       </c>
-      <c r="G46" s="15">
-        <f t="shared" ref="G46" si="2">F46*B46</f>
+      <c r="G47" s="36">
+        <f t="shared" ref="G47" si="2">F47*B47</f>
         <v>130</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H47" s="37">
         <v>10.29</v>
       </c>
-      <c r="J46" s="13"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="35"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-    </row>
-    <row r="48" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E48" s="34" t="s">
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+    </row>
+    <row r="49" spans="5:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="F48" s="34"/>
-      <c r="G48" s="14">
-        <f>SUM(G3:G46)</f>
+      <c r="F49" s="29"/>
+      <c r="G49" s="10">
+        <f>SUM(G3:G47)</f>
         <v>648.57800000000009</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A36:H36"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A48:H48"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
@@ -2606,546 +2747,546 @@
       <selection activeCell="C6" sqref="A6:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.453125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="102.26953125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="4.26953125" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="102.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="18">
-        <v>1</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="14">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="14">
         <v>9</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="14">
         <v>2</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="14">
         <v>2</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="18">
-        <v>1</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="18">
-        <v>1</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="18">
-        <v>1</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="18">
-        <v>1</v>
-      </c>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="14">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="18">
-        <v>1</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17">
+    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <v>732511150</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="18">
-        <v>1</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="18">
-        <v>1</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="16" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="20">
         <v>3</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17" t="s">
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="18">
-        <v>1</v>
-      </c>
-      <c r="E17" s="17" t="s">
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17" t="s">
+    <row r="18" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="18">
-        <v>1</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="14">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24" t="s">
+    <row r="20" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="20">
         <v>7</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17">
+    <row r="21" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>10</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="18">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="D21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="18">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17" t="s">
+      <c r="D22" s="14">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17">
+    <row r="23" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>120</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="14">
         <v>4</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="18">
-        <v>1</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="D24" s="14">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="18" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:5" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="18">
-        <v>1</v>
-      </c>
-      <c r="E25" s="17" t="s">
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="18">
-        <v>1</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="18">
-        <v>1</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="14">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="14">
         <v>2</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17" t="s">
+    <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="18">
-        <v>1</v>
-      </c>
-      <c r="E29" s="17" t="s">
+      <c r="D29" s="14">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="18">
-        <v>1</v>
-      </c>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="14">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="18">
-        <v>1</v>
-      </c>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17" t="s">
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="18">
-        <v>1</v>
-      </c>
-      <c r="E32" s="17" t="s">
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3378,15 +3519,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9f964f78-7045-481f-8f08-bb22d56de14e" xsi:nil="true"/>
@@ -3402,6 +3534,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3424,14 +3565,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F8BD0A9-1453-4AF8-8CA7-9D3A6DF72AF3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3440,4 +3573,12 @@
     <ds:schemaRef ds:uri="59352aba-b979-4180-93b6-1b29a58e7092"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338CEEA-2C13-4615-95BB-3E458545D60E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>